<commit_message>
Homework Part 3 #10
</commit_message>
<xml_diff>
--- a/Section2/ExcelHomework.xlsx
+++ b/Section2/ExcelHomework.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yaw/Code/SavvyCoders/Homework/Section2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82306E73-1DB6-714B-9916-C120BCE9AD84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC5E64B6-CAE0-FF46-9FBD-9CB1BFB4FD69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="58" r:id="rId5"/>
+    <pivotCache cacheId="59" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -727,73 +727,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
-  <dxfs count="17">
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="15">
     <dxf>
       <font>
         <b val="0"/>
@@ -971,17 +905,77 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <top style="thin">
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
           <color indexed="64"/>
-        </top>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -1093,49 +1087,7 @@
           </a:effectLst>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="6"/>
-          <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent1">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -6576,7 +6528,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3BB1D92F-5AE0-AA4B-8AE1-18EC0A2AA08F}" name="PivotTable17" cacheId="58" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3BB1D92F-5AE0-AA4B-8AE1-18EC0A2AA08F}" name="PivotTable17" cacheId="59" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A3:B20" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField numFmtId="14" showAll="0"/>
@@ -6766,10 +6718,10 @@
     <dataField name="Sum of Tax Inclusive Amount" fld="4" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="3">
+    <format dxfId="14">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="1">
+    <format dxfId="13">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
@@ -6797,18 +6749,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4626E862-3B33-E948-930F-1AF5D03AC4FA}" name="ExpensesTable" displayName="ExpensesTable" ref="A2:I210" totalsRowShown="0" headerRowDxfId="4" dataDxfId="5" headerRowBorderDxfId="15" tableBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4626E862-3B33-E948-930F-1AF5D03AC4FA}" name="ExpensesTable" displayName="ExpensesTable" ref="A2:I210" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9">
   <autoFilter ref="A2:I210" xr:uid="{4626E862-3B33-E948-930F-1AF5D03AC4FA}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{FFEDA217-082D-8344-ACB5-EE697BF56A7D}" name="Document Date" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{12B862A5-71F2-134F-9986-F1F1D785912D}" name="Supplier" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{B4107CDB-A5E8-F948-BFC7-EC0B7FD8BBEC}" name="Reference" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{81F83E40-6C36-DB4D-A46E-8558C17C2BDC}" name="Description" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{92613D6C-96DF-6243-9C71-9672D9E51750}" name="Tax Inclusive Amount" dataDxfId="10" dataCellStyle="Comma"/>
-    <tableColumn id="6" xr3:uid="{A4C5202A-195E-B141-8B19-AB5EBA188A3F}" name="Column1" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{0E372207-130F-0047-8A1A-D30BE4A898C6}" name="Bank Code" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{476E5373-D317-5540-B681-32102D7A2242}" name="Account Code" dataDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{639812BB-6C52-524C-A5A7-24263663D9AC}" name="Payment Date" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{FFEDA217-082D-8344-ACB5-EE697BF56A7D}" name="Document Date" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{12B862A5-71F2-134F-9986-F1F1D785912D}" name="Supplier" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{B4107CDB-A5E8-F948-BFC7-EC0B7FD8BBEC}" name="Reference" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{81F83E40-6C36-DB4D-A46E-8558C17C2BDC}" name="Description" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{92613D6C-96DF-6243-9C71-9672D9E51750}" name="Tax Inclusive Amount" dataDxfId="4" dataCellStyle="Comma"/>
+    <tableColumn id="6" xr3:uid="{A4C5202A-195E-B141-8B19-AB5EBA188A3F}" name="Column1" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{0E372207-130F-0047-8A1A-D30BE4A898C6}" name="Bank Code" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{476E5373-D317-5540-B681-32102D7A2242}" name="Account Code" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{639812BB-6C52-524C-A5A7-24263663D9AC}" name="Payment Date" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7113,13 +7065,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA791FAA-07FA-7A4A-A43A-A63E52A275BA}">
   <dimension ref="A3:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B20"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
     <col min="2" max="2" width="16.83203125" style="18" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7277,7 +7229,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I210"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A103" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>

</xml_diff>